<commit_message>
[전인호] NPC데이터 변환, abnomal data수정, grade 수정, Skill 추가
 - armor -> DEF
 - attackspeed -> ATS
 - enemy 삭제
 - mob - Mob
 - cooltime 추가
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Npc.xlsx
+++ b/DesignDocs/VariableData/Npc.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77437D51-E13A-4477-AFCD-8951EB552B15}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175"/>
   </bookViews>
   <sheets>
     <sheet name="Npc" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="91">
   <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -185,10 +184,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>attack_damage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cooltime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -272,10 +267,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>melee</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -304,18 +295,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attackspeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>drop_table</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -324,10 +303,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>armor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -365,13 +340,57 @@
   </si>
   <si>
     <t>Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mob</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -740,15 +759,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.375" customWidth="1"/>
     <col min="8" max="8" width="13.625" customWidth="1"/>
     <col min="10" max="10" width="18.875" bestFit="1" customWidth="1"/>
@@ -774,13 +795,13 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
         <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
       </c>
       <c r="J1" t="s">
         <v>16</v>
@@ -792,22 +813,22 @@
         <v>19</v>
       </c>
       <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" t="s">
-        <v>50</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -827,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -836,13 +857,13 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2">
         <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -857,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="R2" s="1">
         <v>1</v>
@@ -874,13 +895,13 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -889,13 +910,13 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3">
         <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -910,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="R3" s="1">
         <v>1</v>
@@ -921,19 +942,19 @@
         <v>19103</v>
       </c>
       <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
         <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
       </c>
       <c r="F4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -942,13 +963,13 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K4">
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -963,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="R4" s="1">
         <v>1</v>
@@ -977,11 +998,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1070,7 +1091,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
@@ -1081,7 +1102,7 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
@@ -1095,10 +1116,10 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>33</v>
@@ -1109,13 +1130,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -1134,21 +1155,21 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -1162,86 +1183,86 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[전인호] NPC데이터 변환, abnomal data수정, grade 수정, Skill추가     -      armor -> DEF     -       attackspeed -> ATS     -      enemy 삭제     -      mob - MOB    -  cooltime 추가
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Npc.xlsx
+++ b/DesignDocs/VariableData/Npc.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77437D51-E13A-4477-AFCD-8951EB552B15}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175"/>
   </bookViews>
   <sheets>
     <sheet name="Npc" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="91">
   <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -185,10 +184,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>attack_damage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cooltime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -272,10 +267,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>melee</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -304,18 +295,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mob</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attackspeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>drop_table</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -324,10 +303,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>armor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -365,13 +340,57 @@
   </si>
   <si>
     <t>Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mob</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -740,15 +759,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.375" customWidth="1"/>
     <col min="8" max="8" width="13.625" customWidth="1"/>
     <col min="10" max="10" width="18.875" bestFit="1" customWidth="1"/>
@@ -774,13 +795,13 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
         <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
       </c>
       <c r="J1" t="s">
         <v>16</v>
@@ -792,22 +813,22 @@
         <v>19</v>
       </c>
       <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" t="s">
-        <v>50</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -827,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -836,13 +857,13 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2">
         <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -857,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="R2" s="1">
         <v>1</v>
@@ -874,13 +895,13 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -889,13 +910,13 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3">
         <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -910,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="R3" s="1">
         <v>1</v>
@@ -921,19 +942,19 @@
         <v>19103</v>
       </c>
       <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
         <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
       </c>
       <c r="F4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -942,13 +963,13 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K4">
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -963,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="R4" s="1">
         <v>1</v>
@@ -977,11 +998,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1070,7 +1091,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
@@ -1081,7 +1102,7 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
@@ -1095,10 +1116,10 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>33</v>
@@ -1109,13 +1130,13 @@
         <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -1134,21 +1155,21 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -1162,86 +1183,86 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Silverfox] Npc Skill 작업을 위한 Tube 데이터 입력
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Npc.xlsx
+++ b/DesignDocs/VariableData/Npc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A83BD0-8CFF-4361-9AC7-6E414F746F82}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Npc" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
   <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,10 +86,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>melee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>skill</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -249,25 +246,6 @@
   </si>
   <si>
     <t>attack_function</t>
-  </si>
-  <si>
-    <t>attack_function</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nontarget</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{(19_DeadlyAttack)}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{(19_CriticalHit)}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>melee</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -283,18 +261,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>target</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{(19_Badbomb)}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>drop_table</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -343,14 +309,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ATK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>SPD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ATK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ATS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -359,38 +329,66 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SPD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ATS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ATK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mob</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Mob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>style_tube</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enhancer_tube</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cooler_tube</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no107_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no107_enhancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no107_cooler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no108_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no108_enhancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no108_cooler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_enhancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_cooler</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -759,23 +757,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" customWidth="1"/>
-    <col min="8" max="8" width="13.625" customWidth="1"/>
-    <col min="10" max="10" width="18.875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -789,205 +780,133 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="K1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>19101</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
       <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>81</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-      <c r="O2" s="1">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="K2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>19102</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>58</v>
-      </c>
       <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>84</v>
       </c>
       <c r="J3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K3">
-        <v>10</v>
-      </c>
-      <c r="L3" t="s">
-        <v>90</v>
-      </c>
-      <c r="M3" t="b">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>3</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>19103</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
       </c>
       <c r="H4">
         <v>5</v>
       </c>
-      <c r="I4">
-        <v>1</v>
+      <c r="I4" t="s">
+        <v>87</v>
       </c>
       <c r="J4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K4">
-        <v>10</v>
-      </c>
-      <c r="L4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" t="s">
         <v>89</v>
       </c>
-      <c r="M4" t="b">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>5</v>
-      </c>
-      <c r="O4" s="1">
-        <v>1</v>
-      </c>
-      <c r="P4" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R4" s="1">
-        <v>1</v>
+      <c r="L4" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -998,7 +917,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1022,7 +941,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
@@ -1055,7 +974,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -1066,203 +985,203 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
         <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
         <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Silverfox] 논의 전단계 npc skill 체계 마무리
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Npc.xlsx
+++ b/DesignDocs/VariableData/Npc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A83BD0-8CFF-4361-9AC7-6E414F746F82}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883CD1EA-2616-4261-9F86-6149F0417B56}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -337,51 +337,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>style_tube</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enhancer_tube</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cooler_tube</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no107_style</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no107_enhancer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no107_cooler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no108_style</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no108_enhancer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no108_cooler</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jake_style</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jake_enhancer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jake_cooler</t>
+    <t>skill_value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(19_DeadlyAttack)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(19_CriticalHit)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(19_Badbomb)}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -758,15 +726,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -794,17 +762,11 @@
       <c r="I1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>19101</v>
       </c>
@@ -827,19 +789,13 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>19102</v>
       </c>
@@ -862,19 +818,13 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>19103</v>
       </c>
@@ -897,15 +847,9 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J4" t="s">
-        <v>88</v>
-      </c>
-      <c r="K4" t="s">
-        <v>89</v>
-      </c>
-      <c r="L4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[전인호] 몬스터 5종 스킬 완료 No.107, No.108, Jake_B, Jake_R, Doncina
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Npc.xlsx
+++ b/DesignDocs/VariableData/Npc.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B7A434-7316-4780-A0E1-A05695151E82}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175"/>
   </bookViews>
   <sheets>
     <sheet name="Npc" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -253,22 +252,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Jake</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제이크</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>drop_table</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{(19101, 100)}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -345,10 +332,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{(19_Badbomb)}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>nameKor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -362,13 +345,77 @@
   </si>
   <si>
     <t>dropTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jake_B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jake_R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>썩은쥐돌이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엉성한쥐돌이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mob</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(19_jakebounce)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(19_jakerange)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(1100,5),(2100,5),(3100,5)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(1100,5),(2101,5),(3100,5)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(1102,5),(2102,5),(3101,5)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(1101,5),(2101,5),(3102,5)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doncina</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈시나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(19_MustleMustle),(19_HustleHustle)}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{(1103,5),(2100,5),(3101,5),(1101,5),(2101,5),(3100,5),(4101,5)}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -737,14 +784,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -754,7 +807,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -769,18 +822,18 @@
         <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>19101</v>
+        <v>19100</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -789,10 +842,10 @@
         <v>19</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -801,15 +854,15 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>60</v>
+        <v>75</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>19102</v>
+        <v>19101</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -818,10 +871,10 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -830,27 +883,27 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>19103</v>
+        <v>19102</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -859,10 +912,68 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>60</v>
+        <v>86</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>19103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>19200</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -873,11 +984,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -991,7 +1102,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>45</v>
@@ -1033,7 +1144,7 @@
         <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>42</v>
@@ -1086,13 +1197,13 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>56</v>
@@ -1100,13 +1211,13 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>56</v>
@@ -1114,30 +1225,30 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Silverfox] Animset 컬럼 삭제
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Npc.xlsx
+++ b/DesignDocs/VariableData/Npc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3DB2C4-1D16-4FED-BE4B-411AB8D906DE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Npc" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="97">
   <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -415,7 +416,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -784,22 +785,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -810,28 +811,25 @@
         <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="H1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>19100</v>
       </c>
@@ -841,26 +839,26 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <v>50</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>73</v>
       </c>
-      <c r="G2" t="b">
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>19101</v>
       </c>
@@ -870,26 +868,26 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="E3">
+      <c r="D3">
         <v>50</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>74</v>
       </c>
-      <c r="G3" t="b">
+      <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>19102</v>
       </c>
@@ -899,26 +897,26 @@
       <c r="C4" t="s">
         <v>83</v>
       </c>
-      <c r="E4">
+      <c r="D4">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>73</v>
       </c>
-      <c r="G4" t="b">
+      <c r="F4" t="b">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="G4">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" t="s">
         <v>86</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>19103</v>
       </c>
@@ -928,26 +926,26 @@
       <c r="C5" t="s">
         <v>84</v>
       </c>
-      <c r="E5">
+      <c r="D5">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>85</v>
       </c>
-      <c r="G5" t="b">
+      <c r="F5" t="b">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="G5">
         <v>5</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
         <v>87</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>19200</v>
       </c>
@@ -957,22 +955,22 @@
       <c r="C6" t="s">
         <v>93</v>
       </c>
-      <c r="E6">
+      <c r="D6">
         <v>100</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>94</v>
       </c>
-      <c r="G6" t="b">
+      <c r="F6" t="b">
         <v>1</v>
       </c>
-      <c r="H6">
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" t="s">
         <v>95</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>96</v>
       </c>
     </row>
@@ -984,7 +982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
[silverfox] 새 npc 가데이터 입력/
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Npc.xlsx
+++ b/DesignDocs/VariableData/Npc.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChunJ\Desktop\울프팩\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577F7495-D630-42D8-AD5C-7BBC1E5C1906}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11172" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="디스크립션" sheetId="2" r:id="rId1"/>
-    <sheet name="Npc" sheetId="1" r:id="rId2"/>
+    <sheet name="Npc" sheetId="1" r:id="rId1"/>
+    <sheet name="디스크립션" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
   <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -337,14 +338,30 @@
   </si>
   <si>
     <t>고장난 코뱃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cleaner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cleaner_R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클리너</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>깔끔한 클리너</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,13 +377,35 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -383,11 +422,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -703,193 +748,301 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" customWidth="1"/>
+    <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.125" customWidth="1"/>
+    <col min="10" max="10" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="139.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>19100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0.4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B4" s="1" t="s">
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>19101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F3">
+        <v>0.4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>19102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>19103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>19200</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>19104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7">
         <v>70</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>32</v>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>19105</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8">
+        <v>70</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -900,231 +1053,193 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="G13:H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.796875" customWidth="1"/>
-    <col min="8" max="8" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.09765625" customWidth="1"/>
-    <col min="10" max="10" width="36.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="139.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>19100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2">
-        <v>50</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>0.4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>19101</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>0.4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>19102</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4">
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0.5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>19103</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>0.5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>19200</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6">
-        <v>100</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>0.5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
-        <v>50</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>55</v>
+      <c r="E14" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Silverfox] Npc 발주 임시 저장
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Npc.xlsx
+++ b/DesignDocs/VariableData/Npc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9B8A1A-F79B-4F5F-83D0-AACF8EE840FE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDDF064-0D6D-42AC-9EBA-C752C80CD323}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="223">
   <si>
     <t>cid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,13 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>no107_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no107_02</t>
-  </si>
-  <si>
     <t>grade</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -193,14 +186,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Jake_B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jake_R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mob</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -213,14 +198,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>doncina</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>돈시나</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Boss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -337,14 +314,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>고장난 코뱃</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>청소부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">불량한 청소부 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -373,90 +342,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>13_cat_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>의사가운 고양이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13_cat_02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방독면 고양이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13_pitbull</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>핏불 경비원</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>13_owl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>부영이 연구원</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>13_crow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>까마귀 연구원</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>도롱뇽 소각장 인부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13_salamander</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13_carbannog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13_tag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13_tim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13_madbuddy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cleaner</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CleanerR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mingkies</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>18_weasel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>족제비 소매치기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mob</t>
   </si>
   <si>
@@ -491,30 +392,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>닭 불량배</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>닭 칼잡이</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>라쿤 정비공</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>라쿤 용접공</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>17_mole_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>17_mole_02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>17_boar</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -531,22 +408,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>18_camek</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>18_logan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로건</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>카멕</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>두더지 곡괭이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -555,14 +416,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>맷돼지 현장감독</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>박쥐 현장감독</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>거북이 삽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -583,22 +436,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>19_bloom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>19_alliy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>블룸</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>에일리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>16_hyena</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -911,7 +748,167 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>땜장이</t>
+    <t>땜장이 덴틴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중개상 카멕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KoVat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SoVat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소뱃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rat Boy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rat Man</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거대한 싸움꾼 돈시나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현상금 사냥꾼 에일리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황제의 심복 블룸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>깔끔한 청소부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검은 손 스칼렛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cat Doctor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cat Nurse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PitBull Guard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dr Owl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dr Crow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flame Man Salamander</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Carbannog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Officer Tag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Officer Tim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dr.MadBuddy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Great Fighter Don Cena</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Neat Sweep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bad Cleaner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Head Hunter Ailliy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Right-Hand Bloom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>의사 고양이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간호사 고양이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소각장 인부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소매치기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불량배</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>칼잡이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정비공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용접공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현장감독</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mine Worker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dealer Camek</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tinker Dentin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pickpock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black Hand Scarlett</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1379,13 +1376,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.75" customWidth="1"/>
     <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.25" customWidth="1"/>
@@ -1401,31 +1399,31 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1433,10 +1431,10 @@
         <v>19100</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>77</v>
+        <v>186</v>
       </c>
       <c r="D2" s="10">
         <v>50</v>
@@ -1448,7 +1446,7 @@
         <v>0.4</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H2" s="10" t="b">
         <v>1</v>
@@ -1457,10 +1455,10 @@
         <v>3</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1468,10 +1466,10 @@
         <v>19101</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>12</v>
+        <v>184</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D3" s="10">
         <v>50</v>
@@ -1483,7 +1481,7 @@
         <v>0.4</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H3" s="10" t="b">
         <v>1</v>
@@ -1492,10 +1490,10 @@
         <v>3</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1503,10 +1501,10 @@
         <v>19102</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D4" s="10">
         <v>30</v>
@@ -1518,7 +1516,7 @@
         <v>0.5</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4" s="10" t="b">
         <v>1</v>
@@ -1527,10 +1525,10 @@
         <v>5</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1538,10 +1536,10 @@
         <v>19103</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D5" s="10">
         <v>30</v>
@@ -1553,7 +1551,7 @@
         <v>0.5</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H5" s="10" t="b">
         <v>1</v>
@@ -1562,10 +1560,10 @@
         <v>5</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1573,10 +1571,10 @@
         <v>19200</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>47</v>
+        <v>204</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>48</v>
+        <v>189</v>
       </c>
       <c r="D6" s="10">
         <v>100</v>
@@ -1588,19 +1586,19 @@
         <v>0.5</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10">
+        <v>10</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="H6" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="10">
-        <v>10</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1608,10 +1606,10 @@
         <v>19104</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>103</v>
+        <v>205</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>79</v>
+        <v>192</v>
       </c>
       <c r="D7" s="10">
         <v>70</v>
@@ -1623,7 +1621,7 @@
         <v>0.5</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H7" s="10" t="b">
         <v>1</v>
@@ -1632,10 +1630,10 @@
         <v>3</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1643,10 +1641,10 @@
         <v>19105</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>104</v>
+        <v>206</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D8" s="10">
         <v>70</v>
@@ -1658,7 +1656,7 @@
         <v>0.5</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H8" s="10" t="b">
         <v>1</v>
@@ -1667,10 +1665,10 @@
         <v>5</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1678,10 +1676,10 @@
         <v>19106</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D9" s="10">
         <v>50</v>
@@ -1693,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H9" s="10" t="b">
         <v>1</v>
@@ -1702,10 +1700,10 @@
         <v>30</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1713,10 +1711,10 @@
         <v>19107</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>141</v>
+        <v>208</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="D10" s="10">
         <v>100</v>
@@ -1728,19 +1726,19 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <v>10</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="H10" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="10">
-        <v>10</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1748,10 +1746,10 @@
         <v>19108</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>142</v>
+        <v>207</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="D11" s="10">
         <v>100</v>
@@ -1763,19 +1761,19 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10">
+        <v>10</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="H11" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="10">
-        <v>10</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1783,10 +1781,10 @@
         <v>13100</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>87</v>
+        <v>194</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>88</v>
+        <v>209</v>
       </c>
       <c r="D12" s="2">
         <v>30</v>
@@ -1798,7 +1796,7 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H12" s="2" t="b">
         <v>1</v>
@@ -1807,10 +1805,10 @@
         <v>5</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1818,10 +1816,10 @@
         <v>13101</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>89</v>
+        <v>195</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>90</v>
+        <v>210</v>
       </c>
       <c r="D13" s="2">
         <v>30</v>
@@ -1833,7 +1831,7 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H13" s="2" t="b">
         <v>1</v>
@@ -1842,10 +1840,10 @@
         <v>5</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1853,10 +1851,10 @@
         <v>13102</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>91</v>
+        <v>196</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D14" s="2">
         <v>30</v>
@@ -1868,7 +1866,7 @@
         <v>0.5</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H14" s="2" t="b">
         <v>1</v>
@@ -1877,10 +1875,10 @@
         <v>5</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1888,10 +1886,10 @@
         <v>13103</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>93</v>
+        <v>197</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D15" s="2">
         <v>30</v>
@@ -1903,7 +1901,7 @@
         <v>0.5</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H15" s="2" t="b">
         <v>1</v>
@@ -1912,10 +1910,10 @@
         <v>5</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1923,10 +1921,10 @@
         <v>13104</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>95</v>
+        <v>198</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D16" s="2">
         <v>30</v>
@@ -1938,7 +1936,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H16" s="2" t="b">
         <v>1</v>
@@ -1947,10 +1945,10 @@
         <v>5</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1958,10 +1956,10 @@
         <v>13105</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>98</v>
+        <v>199</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>211</v>
       </c>
       <c r="D17" s="2">
         <v>30</v>
@@ -1973,7 +1971,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H17" s="2" t="b">
         <v>1</v>
@@ -1982,10 +1980,10 @@
         <v>5</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1993,10 +1991,10 @@
         <v>13106</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>99</v>
+        <v>200</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>212</v>
+        <v>171</v>
       </c>
       <c r="D18" s="2">
         <v>100</v>
@@ -2008,19 +2006,19 @@
         <v>0.5</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>10</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="H18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="2">
-        <v>10</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2028,10 +2026,10 @@
         <v>13107</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>100</v>
+        <v>201</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>213</v>
+        <v>172</v>
       </c>
       <c r="D19" s="2">
         <v>100</v>
@@ -2043,19 +2041,19 @@
         <v>0.5</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>10</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="H19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2">
-        <v>10</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2063,10 +2061,10 @@
         <v>13108</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
       <c r="D20" s="2">
         <v>100</v>
@@ -2078,19 +2076,19 @@
         <v>0.5</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>10</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="H20" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2">
-        <v>10</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2098,10 +2096,10 @@
         <v>13109</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>102</v>
+        <v>203</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>215</v>
+        <v>174</v>
       </c>
       <c r="D21" s="2">
         <v>100</v>
@@ -2113,19 +2111,19 @@
         <v>0.5</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>10</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="H21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2">
-        <v>10</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2133,10 +2131,10 @@
         <v>18100</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>106</v>
+        <v>221</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>107</v>
+        <v>212</v>
       </c>
       <c r="D22" s="3">
         <v>30</v>
@@ -2148,7 +2146,7 @@
         <v>0.5</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H22" s="3" t="b">
         <v>1</v>
@@ -2157,10 +2155,10 @@
         <v>5</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2168,10 +2166,10 @@
         <v>18101</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>118</v>
+        <v>213</v>
       </c>
       <c r="D23" s="3">
         <v>30</v>
@@ -2183,7 +2181,7 @@
         <v>0.5</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H23" s="3" t="b">
         <v>1</v>
@@ -2192,10 +2190,10 @@
         <v>5</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2203,10 +2201,10 @@
         <v>18102</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="D24" s="3">
         <v>30</v>
@@ -2218,7 +2216,7 @@
         <v>0.5</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H24" s="3" t="b">
         <v>1</v>
@@ -2227,10 +2225,10 @@
         <v>5</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2238,10 +2236,10 @@
         <v>18103</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>120</v>
+        <v>215</v>
       </c>
       <c r="D25" s="3">
         <v>30</v>
@@ -2253,7 +2251,7 @@
         <v>0.5</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H25" s="3" t="b">
         <v>1</v>
@@ -2262,10 +2260,10 @@
         <v>5</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2273,10 +2271,10 @@
         <v>18104</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>121</v>
+        <v>216</v>
       </c>
       <c r="D26" s="3">
         <v>30</v>
@@ -2288,7 +2286,7 @@
         <v>0.5</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H26" s="3" t="b">
         <v>1</v>
@@ -2297,10 +2295,10 @@
         <v>5</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2308,10 +2306,10 @@
         <v>18105</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>129</v>
+        <v>222</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="D27" s="3">
         <v>100</v>
@@ -2323,7 +2321,7 @@
         <v>0.5</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H27" s="3" t="b">
         <v>1</v>
@@ -2332,10 +2330,10 @@
         <v>10</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2343,10 +2341,10 @@
         <v>18106</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>128</v>
+        <v>219</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>131</v>
+        <v>183</v>
       </c>
       <c r="D28" s="3">
         <v>100</v>
@@ -2358,7 +2356,7 @@
         <v>0.5</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H28" s="3" t="b">
         <v>1</v>
@@ -2367,21 +2365,21 @@
         <v>10</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>18107</v>
       </c>
-      <c r="B29" s="3">
-        <v>18</v>
+      <c r="B29" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>223</v>
+        <v>182</v>
       </c>
       <c r="D29" s="3">
         <v>100</v>
@@ -2393,7 +2391,7 @@
         <v>0.5</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H29" s="3" t="b">
         <v>1</v>
@@ -2402,10 +2400,10 @@
         <v>10</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2413,10 +2411,10 @@
         <v>17100</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>122</v>
+        <v>218</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="D30" s="4">
         <v>30</v>
@@ -2428,7 +2426,7 @@
         <v>0.5</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H30" s="4" t="b">
         <v>1</v>
@@ -2437,10 +2435,10 @@
         <v>5</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2448,10 +2446,10 @@
         <v>17101</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>123</v>
+        <v>218</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="D31" s="4">
         <v>30</v>
@@ -2463,7 +2461,7 @@
         <v>0.5</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H31" s="4" t="b">
         <v>1</v>
@@ -2472,10 +2470,10 @@
         <v>5</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2483,10 +2481,10 @@
         <v>17102</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>134</v>
+        <v>217</v>
       </c>
       <c r="D32" s="4">
         <v>30</v>
@@ -2498,7 +2496,7 @@
         <v>0.5</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H32" s="4" t="b">
         <v>1</v>
@@ -2507,10 +2505,10 @@
         <v>5</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2518,10 +2516,10 @@
         <v>17103</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>135</v>
+        <v>217</v>
       </c>
       <c r="D33" s="4">
         <v>30</v>
@@ -2533,7 +2531,7 @@
         <v>0.5</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H33" s="4" t="b">
         <v>1</v>
@@ -2542,10 +2540,10 @@
         <v>5</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2553,10 +2551,10 @@
         <v>17104</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="D34" s="4">
         <v>30</v>
@@ -2568,7 +2566,7 @@
         <v>0.5</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H34" s="4" t="b">
         <v>1</v>
@@ -2577,10 +2575,10 @@
         <v>5</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2588,10 +2586,10 @@
         <v>17105</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="D35" s="4">
         <v>30</v>
@@ -2603,7 +2601,7 @@
         <v>0.5</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H35" s="4" t="b">
         <v>1</v>
@@ -2612,10 +2610,10 @@
         <v>5</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2623,10 +2621,10 @@
         <v>17106</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>168</v>
+        <v>127</v>
       </c>
       <c r="D36" s="4">
         <v>100</v>
@@ -2638,7 +2636,7 @@
         <v>0.5</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H36" s="4" t="b">
         <v>1</v>
@@ -2647,10 +2645,10 @@
         <v>10</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2658,10 +2656,10 @@
         <v>17107</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="D37" s="4">
         <v>100</v>
@@ -2673,7 +2671,7 @@
         <v>0.5</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H37" s="4" t="b">
         <v>1</v>
@@ -2682,10 +2680,10 @@
         <v>10</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -2693,10 +2691,10 @@
         <v>17108</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="D38" s="4">
         <v>100</v>
@@ -2708,7 +2706,7 @@
         <v>0.5</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H38" s="4" t="b">
         <v>1</v>
@@ -2717,10 +2715,10 @@
         <v>10</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2728,10 +2726,10 @@
         <v>16100</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="D39" s="6">
         <v>30</v>
@@ -2743,7 +2741,7 @@
         <v>0.5</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H39" s="6" t="b">
         <v>1</v>
@@ -2752,10 +2750,10 @@
         <v>5</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2763,10 +2761,10 @@
         <v>16101</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
       <c r="D40" s="6">
         <v>30</v>
@@ -2778,7 +2776,7 @@
         <v>0.5</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H40" s="6" t="b">
         <v>1</v>
@@ -2787,10 +2785,10 @@
         <v>5</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2798,10 +2796,10 @@
         <v>16102</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="D41" s="6">
         <v>30</v>
@@ -2813,7 +2811,7 @@
         <v>0.5</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H41" s="6" t="b">
         <v>1</v>
@@ -2822,10 +2820,10 @@
         <v>5</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2833,10 +2831,10 @@
         <v>16103</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="D42" s="6">
         <v>30</v>
@@ -2848,7 +2846,7 @@
         <v>0.5</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H42" s="6" t="b">
         <v>1</v>
@@ -2857,10 +2855,10 @@
         <v>5</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2868,10 +2866,10 @@
         <v>16104</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D43" s="6">
         <v>30</v>
@@ -2883,7 +2881,7 @@
         <v>0.5</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H43" s="6" t="b">
         <v>1</v>
@@ -2892,10 +2890,10 @@
         <v>5</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2903,10 +2901,10 @@
         <v>16105</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="D44" s="6">
         <v>100</v>
@@ -2918,7 +2916,7 @@
         <v>0.5</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H44" s="6" t="b">
         <v>1</v>
@@ -2927,10 +2925,10 @@
         <v>10</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2938,10 +2936,10 @@
         <v>16106</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="D45" s="6">
         <v>100</v>
@@ -2953,7 +2951,7 @@
         <v>0.5</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H45" s="6" t="b">
         <v>1</v>
@@ -2962,10 +2960,10 @@
         <v>10</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2973,10 +2971,10 @@
         <v>16107</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="D46" s="6">
         <v>100</v>
@@ -2988,7 +2986,7 @@
         <v>0.5</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H46" s="6" t="b">
         <v>1</v>
@@ -2997,10 +2995,10 @@
         <v>10</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3008,10 +3006,10 @@
         <v>15100</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="D47" s="5">
         <v>30</v>
@@ -3023,7 +3021,7 @@
         <v>0.5</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H47" s="5" t="b">
         <v>1</v>
@@ -3032,10 +3030,10 @@
         <v>5</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3043,10 +3041,10 @@
         <v>15101</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>159</v>
+        <v>118</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="D48" s="5">
         <v>30</v>
@@ -3058,7 +3056,7 @@
         <v>0.5</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H48" s="5" t="b">
         <v>1</v>
@@ -3067,10 +3065,10 @@
         <v>5</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3078,10 +3076,10 @@
         <v>15102</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="D49" s="5">
         <v>30</v>
@@ -3093,7 +3091,7 @@
         <v>0.5</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H49" s="5" t="b">
         <v>1</v>
@@ -3102,10 +3100,10 @@
         <v>5</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3113,10 +3111,10 @@
         <v>15103</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="D50" s="5">
         <v>100</v>
@@ -3128,7 +3126,7 @@
         <v>0.5</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H50" s="5" t="b">
         <v>1</v>
@@ -3137,10 +3135,10 @@
         <v>10</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3148,10 +3146,10 @@
         <v>15104</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="D51" s="5">
         <v>100</v>
@@ -3163,7 +3161,7 @@
         <v>0.5</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H51" s="5" t="b">
         <v>1</v>
@@ -3172,10 +3170,10 @@
         <v>10</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3183,10 +3181,10 @@
         <v>14100</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>169</v>
+        <v>128</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
       <c r="D52" s="7">
         <v>30</v>
@@ -3198,7 +3196,7 @@
         <v>0.5</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H52" s="7" t="b">
         <v>1</v>
@@ -3207,10 +3205,10 @@
         <v>5</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3218,10 +3216,10 @@
         <v>14101</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="D53" s="7">
         <v>30</v>
@@ -3233,7 +3231,7 @@
         <v>0.5</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H53" s="7" t="b">
         <v>1</v>
@@ -3242,10 +3240,10 @@
         <v>5</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3253,10 +3251,10 @@
         <v>14102</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="D54" s="7">
         <v>30</v>
@@ -3268,7 +3266,7 @@
         <v>0.5</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H54" s="7" t="b">
         <v>1</v>
@@ -3277,10 +3275,10 @@
         <v>5</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3288,10 +3286,10 @@
         <v>14103</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="D55" s="7">
         <v>30</v>
@@ -3303,7 +3301,7 @@
         <v>0.5</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H55" s="7" t="b">
         <v>1</v>
@@ -3312,10 +3310,10 @@
         <v>5</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K55" s="7" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3323,10 +3321,10 @@
         <v>14104</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="D56" s="7">
         <v>30</v>
@@ -3338,7 +3336,7 @@
         <v>0.5</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H56" s="7" t="b">
         <v>1</v>
@@ -3347,10 +3345,10 @@
         <v>5</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3358,10 +3356,10 @@
         <v>14105</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="D57" s="7">
         <v>100</v>
@@ -3373,7 +3371,7 @@
         <v>0.5</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H57" s="7" t="b">
         <v>1</v>
@@ -3382,10 +3380,10 @@
         <v>10</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K57" s="7" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3393,10 +3391,10 @@
         <v>14106</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>181</v>
+        <v>140</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="D58" s="7">
         <v>100</v>
@@ -3408,7 +3406,7 @@
         <v>0.5</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H58" s="7" t="b">
         <v>1</v>
@@ -3417,10 +3415,10 @@
         <v>10</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K58" s="7" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3428,10 +3426,10 @@
         <v>14107</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="D59" s="7">
         <v>100</v>
@@ -3443,7 +3441,7 @@
         <v>0.5</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H59" s="7" t="b">
         <v>1</v>
@@ -3452,10 +3450,10 @@
         <v>10</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3463,10 +3461,10 @@
         <v>14108</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="D60" s="7">
         <v>100</v>
@@ -3478,7 +3476,7 @@
         <v>0.5</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H60" s="7" t="b">
         <v>1</v>
@@ -3487,10 +3485,10 @@
         <v>10</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K60" s="7" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3498,10 +3496,10 @@
         <v>14109</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="D61" s="7">
         <v>100</v>
@@ -3513,7 +3511,7 @@
         <v>0.5</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H61" s="7" t="b">
         <v>1</v>
@@ -3522,10 +3520,10 @@
         <v>10</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K61" s="7" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3533,10 +3531,10 @@
         <v>14110</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>190</v>
+        <v>149</v>
       </c>
       <c r="D62" s="7">
         <v>100</v>
@@ -3548,7 +3546,7 @@
         <v>0.5</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H62" s="7" t="b">
         <v>1</v>
@@ -3557,10 +3555,10 @@
         <v>10</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K62" s="7" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -3568,10 +3566,10 @@
         <v>14111</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
       <c r="D63" s="7">
         <v>100</v>
@@ -3583,7 +3581,7 @@
         <v>0.5</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H63" s="7" t="b">
         <v>1</v>
@@ -3592,10 +3590,10 @@
         <v>10</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K63" s="7" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3603,10 +3601,10 @@
         <v>13100</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>174</v>
+        <v>133</v>
       </c>
       <c r="D64" s="9">
         <v>30</v>
@@ -3618,7 +3616,7 @@
         <v>0.5</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H64" s="9" t="b">
         <v>1</v>
@@ -3627,10 +3625,10 @@
         <v>5</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3638,10 +3636,10 @@
         <v>13101</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>195</v>
+        <v>154</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>202</v>
+        <v>161</v>
       </c>
       <c r="D65" s="9">
         <v>30</v>
@@ -3653,7 +3651,7 @@
         <v>0.5</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H65" s="9" t="b">
         <v>1</v>
@@ -3662,10 +3660,10 @@
         <v>5</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3673,10 +3671,10 @@
         <v>13102</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>203</v>
+        <v>162</v>
       </c>
       <c r="D66" s="9">
         <v>30</v>
@@ -3688,7 +3686,7 @@
         <v>0.5</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H66" s="9" t="b">
         <v>1</v>
@@ -3697,10 +3695,10 @@
         <v>5</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3708,10 +3706,10 @@
         <v>13103</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>196</v>
+        <v>155</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>197</v>
+        <v>156</v>
       </c>
       <c r="D67" s="9">
         <v>30</v>
@@ -3723,7 +3721,7 @@
         <v>0.5</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H67" s="9" t="b">
         <v>1</v>
@@ -3732,10 +3730,10 @@
         <v>5</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3743,10 +3741,10 @@
         <v>13104</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>198</v>
+        <v>157</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>199</v>
+        <v>158</v>
       </c>
       <c r="D68" s="9">
         <v>100</v>
@@ -3758,7 +3756,7 @@
         <v>0.5</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H68" s="9" t="b">
         <v>1</v>
@@ -3767,10 +3765,10 @@
         <v>10</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K68" s="9" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3778,10 +3776,10 @@
         <v>13105</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>200</v>
+        <v>159</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>201</v>
+        <v>160</v>
       </c>
       <c r="D69" s="9">
         <v>100</v>
@@ -3793,7 +3791,7 @@
         <v>0.5</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H69" s="9" t="b">
         <v>1</v>
@@ -3802,10 +3800,10 @@
         <v>10</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K69" s="9" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -3813,10 +3811,10 @@
         <v>12100</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>204</v>
+        <v>163</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>211</v>
+        <v>170</v>
       </c>
       <c r="D70" s="8">
         <v>30</v>
@@ -3828,7 +3826,7 @@
         <v>0.5</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H70" s="8" t="b">
         <v>1</v>
@@ -3837,10 +3835,10 @@
         <v>5</v>
       </c>
       <c r="J70" s="8" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K70" s="8" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -3848,10 +3846,10 @@
         <v>12101</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>209</v>
+        <v>168</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="D71" s="8">
         <v>30</v>
@@ -3863,7 +3861,7 @@
         <v>0.5</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H71" s="8" t="b">
         <v>1</v>
@@ -3872,10 +3870,10 @@
         <v>5</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="K71" s="8" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -3883,10 +3881,10 @@
         <v>12102</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>205</v>
+        <v>164</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>207</v>
+        <v>166</v>
       </c>
       <c r="D72" s="8">
         <v>100</v>
@@ -3898,7 +3896,7 @@
         <v>0.5</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H72" s="8" t="b">
         <v>1</v>
@@ -3907,10 +3905,10 @@
         <v>10</v>
       </c>
       <c r="J72" s="8" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -3918,10 +3916,10 @@
         <v>12103</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>206</v>
+        <v>165</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="D73" s="8">
         <v>100</v>
@@ -3933,7 +3931,7 @@
         <v>0.5</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H73" s="8" t="b">
         <v>1</v>
@@ -3942,10 +3940,10 @@
         <v>10</v>
       </c>
       <c r="J73" s="8" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -3953,10 +3951,10 @@
         <v>12103</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>221</v>
+        <v>180</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>222</v>
+        <v>181</v>
       </c>
       <c r="D74" s="8">
         <v>100</v>
@@ -3968,7 +3966,7 @@
         <v>0.5</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="H74" s="8" t="b">
         <v>1</v>
@@ -3977,10 +3975,10 @@
         <v>10</v>
       </c>
       <c r="J74" s="8" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -4015,12 +4013,12 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -4050,134 +4048,134 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Silverfox] 로프/트랩 기믹 발주 문서 , NPC Cid 정리, Text Box 더미 등록
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/Npc.xlsx
+++ b/DesignDocs/VariableData/Npc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906A6175-5C83-4529-83B9-18970E0049C8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D8CC58-A197-4825-AC3D-9D2EEC48C45E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1376,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1682,7 +1682,7 @@
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>13100</v>
+        <v>14100</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>184</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>13101</v>
+        <v>14101</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>185</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>13102</v>
+        <v>14102</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>186</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>13103</v>
+        <v>14103</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>187</v>
@@ -1786,7 +1786,7 @@
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>13104</v>
+        <v>14104</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>188</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>13105</v>
+        <v>14105</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>189</v>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>13106</v>
+        <v>14106</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>190</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>13107</v>
+        <v>14107</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>191</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>13108</v>
+        <v>14108</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>192</v>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>13109</v>
+        <v>14109</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>193</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="52" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
-        <v>14100</v>
+        <v>13100</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>118</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="53" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
-        <v>14101</v>
+        <v>13101</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>120</v>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="54" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
-        <v>14102</v>
+        <v>13102</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>122</v>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="55" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
-        <v>14103</v>
+        <v>13103</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>124</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="56" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
-        <v>14104</v>
+        <v>13104</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>126</v>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="57" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
-        <v>14105</v>
+        <v>13105</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>128</v>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="58" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
-        <v>14106</v>
+        <v>13106</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>130</v>
@@ -2904,7 +2904,7 @@
     </row>
     <row r="59" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
-        <v>14107</v>
+        <v>13107</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>132</v>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="60" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
-        <v>14108</v>
+        <v>13108</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>134</v>
@@ -2956,7 +2956,7 @@
     </row>
     <row r="61" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
-        <v>14109</v>
+        <v>13109</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>136</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="62" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
-        <v>14110</v>
+        <v>13110</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>138</v>
@@ -3008,7 +3008,7 @@
     </row>
     <row r="63" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
-        <v>14111</v>
+        <v>13111</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>140</v>
@@ -3034,7 +3034,7 @@
     </row>
     <row r="64" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="9">
-        <v>13100</v>
+        <v>12100</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>143</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="65" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9">
-        <v>13101</v>
+        <v>12101</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>144</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="66" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
-        <v>13102</v>
+        <v>12102</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>142</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="67" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="9">
-        <v>13103</v>
+        <v>12103</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>145</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="68" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="9">
-        <v>13104</v>
+        <v>12104</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>147</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="69" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="9">
-        <v>13105</v>
+        <v>12105</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>149</v>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="70" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="8">
-        <v>12100</v>
+        <v>11100</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>153</v>
@@ -3216,7 +3216,7 @@
     </row>
     <row r="71" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8">
-        <v>12101</v>
+        <v>11101</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>158</v>
@@ -3242,7 +3242,7 @@
     </row>
     <row r="72" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8">
-        <v>12102</v>
+        <v>11102</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>154</v>
@@ -3268,7 +3268,7 @@
     </row>
     <row r="73" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8">
-        <v>12103</v>
+        <v>11103</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>155</v>
@@ -3294,7 +3294,7 @@
     </row>
     <row r="74" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8">
-        <v>12103</v>
+        <v>11104</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>170</v>

</xml_diff>